<commit_message>
Updated as of May 30, 2022
</commit_message>
<xml_diff>
--- a/Mitigation implementations timelines.xlsx
+++ b/Mitigation implementations timelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Documents/GitHub/CovidPolicy-Canada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CF50AE-0819-A246-8C64-5D8410EFE066}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BB213A-F858-DA4E-87D2-FC3ED33506C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12800" yWindow="520" windowWidth="15280" windowHeight="15900" firstSheet="7" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10924,10 +10924,6 @@
     <t>04/04/2022</t>
   </si>
   <si>
-    <t>Vaccine mandate is fully lifted but it will continue to be required for employees, contractors and volunteers working in high-risk settings in the Yukon.
-High-risk settings include: long-term care homes; residential substance use programs; hospitals; shelters; residential care for children and adults; correctional centres; Yukon government-operated community health centres; and Yukon government-operated public health clinics, including the referred care clinic. (https://yukon.ca/en/news/vaccination-requirement-continues-workers-high-risk-settings-yukon) (https://yukon.ca/en/news/vaccination-requirement-lifted-most-workers)</t>
-  </si>
-  <si>
     <t>There are no longer any gathering limits or capacity limits
  Physical distancing is no longer required between people and groups
  Masks are no longer required in most indoor public places, including restaurants, theatres and stores; Masks are still required in health-care settings, long-term care homes, adult residential centres, and other high-risk settings, such as provincial jails. Masks are also mandatory in public schools and school buses. 
@@ -10995,6 +10991,10 @@
     <t>The public health order requiring mandatory indoor masking and self-isolation for anyone who tests positive for COVID-19 through a PCR or at-home rapid antigen test is no longer in effect as of 12:01 a.m. February 28.Public Health still strongly recommends immediate self-isolation for anyone who tests positive for COVID-19.
 Businesses, workplaces and event organizers may request that patrons/visitors/staff/students continue to mask. Masking will not be mandatory. (https://www.saskatchewan.ca/government/health-care-administration-and-provider-resources/treatment-procedures-and-guidelines/emerging-public-health-issues/2019-novel-coronavirus/public-health-measures). As of February 28 2022, non-medical masks  will continue to be required when traveling on Saskatoon Transit vehicles. 
 This applies to all customers, including those who have been vaccinated. (https://transit.saskatoon.ca/rider-guide/covid-19/face-masks)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccine mandate is fully lifted but it will continue to be required for employees, contractors and volunteers working in high-risk settings in the Yukon.
+High-risk settings include: long-term care homes; residential substance use programs; hospitals; shelters; residential care for children and adults; correctional centres; Yukon government-operated community health centres; and Yukon government-operated public health clinics, including the referred care clinic. (https://yukon.ca/en/news/vaccination-requirement-continues-workers-high-risk-settings-yukon) (https://yukon.ca/en/news/vaccination-requirement-lifted-most-workers) </t>
   </si>
 </sst>
 </file>
@@ -12892,23 +12892,23 @@
         <v>1172</v>
       </c>
       <c r="B67" s="166" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="51">
       <c r="A68" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B68" s="169" t="s">
         <v>1225</v>
-      </c>
-      <c r="B68" s="169" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="34">
       <c r="A69" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B69" s="169" t="s">
         <v>1227</v>
-      </c>
-      <c r="B69" s="169" t="s">
-        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -13690,10 +13690,10 @@
     </row>
     <row r="38" spans="1:2" ht="51">
       <c r="A38" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B38" s="169" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
     </row>
   </sheetData>
@@ -13980,10 +13980,10 @@
     </row>
     <row r="33" spans="1:2" s="170" customFormat="1" ht="34">
       <c r="A33" s="1" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B33" s="171" t="s">
         <v>1234</v>
-      </c>
-      <c r="B33" s="171" t="s">
-        <v>1235</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="85">
@@ -13991,15 +13991,15 @@
         <v>1214</v>
       </c>
       <c r="B34" s="166" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="68">
       <c r="A35" s="1" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="B35" s="169" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
     </row>
   </sheetData>
@@ -14908,7 +14908,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="255">
+    <row r="27" spans="1:3" ht="272">
       <c r="A27" s="6" t="s">
         <v>164</v>
       </c>
@@ -15147,7 +15147,7 @@
         <v>1193</v>
       </c>
       <c r="B54" s="166" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
     </row>
   </sheetData>
@@ -15741,7 +15741,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="136">
+    <row r="8" spans="1:3" ht="153">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -16016,10 +16016,10 @@
     </row>
     <row r="41" spans="1:3" s="174" customFormat="1" ht="170">
       <c r="A41" s="6" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>1236</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>1237</v>
       </c>
       <c r="C41" s="175"/>
     </row>
@@ -16028,7 +16028,7 @@
         <v>1170</v>
       </c>
       <c r="B42" s="46" t="s">
-        <v>1233</v>
+        <v>1232</v>
       </c>
       <c r="C42" s="90" t="s">
         <v>227</v>
@@ -16995,7 +16995,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="120" customFormat="1" ht="136">
+    <row r="111" spans="1:3" s="120" customFormat="1" ht="153">
       <c r="A111" s="6" t="s">
         <v>1051</v>
       </c>
@@ -18765,7 +18765,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -19054,7 +19054,7 @@
         <v>1222</v>
       </c>
       <c r="B35" s="172" t="s">
-        <v>1223</v>
+        <v>1237</v>
       </c>
     </row>
   </sheetData>

</xml_diff>